<commit_message>
Avance 1 de base de datos
</commit_message>
<xml_diff>
--- a/docs/Ventas_DB.xlsx
+++ b/docs/Ventas_DB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\TECMM\PROYECTO FINAL\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\TECMM\PROYECTO FINAL\PuntoVentas\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45769B2-C239-434F-AA6D-DB89814A4F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46709282-4DB3-4466-A0B0-D11FF3F9D8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EFD8329D-E457-41A7-97B0-A32A3BAA043E}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>id_provedor</t>
   </si>
   <si>
-    <t>Provedores</t>
-  </si>
-  <si>
     <t>id_producto</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>nombre_producto</t>
   </si>
   <si>
-    <t>fecha_de_registro</t>
-  </si>
-  <si>
     <t>Productos</t>
   </si>
   <si>
@@ -135,6 +129,12 @@
   </si>
   <si>
     <t>foto_usuario</t>
+  </si>
+  <si>
+    <t>fecha_registro</t>
+  </si>
+  <si>
+    <t>Proveedores</t>
   </si>
 </sst>
 </file>
@@ -167,12 +167,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -239,9 +245,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -251,11 +258,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999811C4-DF84-4502-8DBE-496C91E62BF7}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -609,176 +624,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="B11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="C11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>32</v>
+      <c r="F11" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terminacion de Base de Datos
</commit_message>
<xml_diff>
--- a/docs/Ventas_DB.xlsx
+++ b/docs/Ventas_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\TECMM\PROYECTO FINAL\PuntoVentas\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46709282-4DB3-4466-A0B0-D11FF3F9D8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ADF427-8329-4B46-A4A0-77C2CDA86117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EFD8329D-E457-41A7-97B0-A32A3BAA043E}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{EFD8329D-E457-41A7-97B0-A32A3BAA043E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>nombre_contacto</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Productos</t>
   </si>
   <si>
-    <t>id_productos</t>
-  </si>
-  <si>
     <t>tipo</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Proveedores</t>
+  </si>
+  <si>
+    <t>fecha_inventario</t>
   </si>
 </sst>
 </file>
@@ -245,17 +245,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -265,10 +259,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -607,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999811C4-DF84-4502-8DBE-496C91E62BF7}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -624,176 +614,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="F8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="G14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -802,8 +796,8 @@
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A7:E7"/>
     <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>